<commit_message>
Update database Excel files
</commit_message>
<xml_diff>
--- a/backend/database/PostgreSQL-persons.xlsx
+++ b/backend/database/PostgreSQL-persons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="create-persons" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t xml:space="preserve">CREATE TABLE </t>
   </si>
@@ -89,9 +89,6 @@
     <t>updated_at</t>
   </si>
   <si>
-    <t>NOT NULL</t>
-  </si>
-  <si>
     <t>SERIAL PRIMARY KEY,</t>
   </si>
   <si>
@@ -113,13 +110,22 @@
     <t>INSERT INTO persons VALUES (999, 'chefedegabinete@senado.leg.br', 'Chefe', 'de Gabinete', '9999', 'SF', null, 'C');</t>
   </si>
   <si>
-    <t>INSERT INTO private.accounts VALUES (1, crypt('123456', gen_salt('bf', 10)), '2019-08-01', '2019-08-02');</t>
-  </si>
-  <si>
-    <t>INSERT INTO private.accounts VALUES (2, crypt('123456', gen_salt('bf', 10)), '2019-08-01', '2019-08-02');</t>
-  </si>
-  <si>
-    <t>INSERT INTO private.accounts VALUES (3, crypt('123456', gen_salt('bf', 10)), '2019-08-01', '2019-08-02');</t>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>NOT NULL DEFAULT true</t>
+  </si>
+  <si>
+    <t>INSERT INTO private.accounts VALUES (1, crypt('123456', gen_salt('bf', 10)), '2019-08-01', '2019-08-02', true);</t>
+  </si>
+  <si>
+    <t>INSERT INTO private.accounts VALUES (2, crypt('123456', gen_salt('bf', 10)), '2019-08-01', '2019-08-02', true);</t>
+  </si>
+  <si>
+    <t>INSERT INTO private.accounts VALUES (3, crypt('123456', gen_salt('bf', 10)), '2019-08-01', '2019-08-02', true);</t>
   </si>
 </sst>
 </file>
@@ -619,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>16</v>
@@ -633,7 +639,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,10 +730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +769,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -791,17 +797,28 @@
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -814,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -825,37 +842,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>